<commit_message>
Se agrega prueba de periodo 2
</commit_message>
<xml_diff>
--- a/Resultados_Simulacro_ICFES.xlsx
+++ b/Resultados_Simulacro_ICFES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Project_Python\rs_icfes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\COMPUMAX\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5372B073-3EEA-49E6-B9AB-B345D0380893}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B5F0548-2A7E-434B-8F53-41052E70CF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E084411A-0BE6-4F73-A93C-EC29D2242342}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E084411A-0BE6-4F73-A93C-EC29D2242342}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2067" uniqueCount="463">
   <si>
     <t>Grupo</t>
   </si>
@@ -1276,13 +1276,154 @@
   </si>
   <si>
     <t>1106</t>
+  </si>
+  <si>
+    <t>ARAUJO CAMACARO, JORGE ALEJANDRO</t>
+  </si>
+  <si>
+    <t>ARIAS OCHOA, MICHAEL YAIR</t>
+  </si>
+  <si>
+    <t>BALLESTEROS JARAMILLO, ANA SOFIA</t>
+  </si>
+  <si>
+    <t>CABRERA SALAZAR, ESTEFANIA</t>
+  </si>
+  <si>
+    <t>CASTRILLON UPEGUI, BRANDON</t>
+  </si>
+  <si>
+    <t>CHAVARRIAGA AGUDELO, CARLOS DUVAN</t>
+  </si>
+  <si>
+    <t>COLMENAREZ MARTINEZ, ISABEL YENIRE</t>
+  </si>
+  <si>
+    <t>CORDOVA MAESTRE, DARIANNA JEIMILY</t>
+  </si>
+  <si>
+    <t>DURAN BERMUDEZ, ROBERT IGNACIO</t>
+  </si>
+  <si>
+    <t>GALLEGO PINO, LEYDI YULIANA</t>
+  </si>
+  <si>
+    <t>GARCIA TORRES, SAMUEL</t>
+  </si>
+  <si>
+    <t>GIRALDO CHICA, MARIA PAULINA</t>
+  </si>
+  <si>
+    <t>GIRALDO HENAO, MARIA JOSE</t>
+  </si>
+  <si>
+    <t>INFANTE SAGANOME, MIGUEL ANGEL</t>
+  </si>
+  <si>
+    <t>LOPEZ ALVAREZ, ANDERSON</t>
+  </si>
+  <si>
+    <t>MARCANO MENDEZ, AARLON DAVID</t>
+  </si>
+  <si>
+    <t>MOLINA MEJIA, JUAN DIEGO</t>
+  </si>
+  <si>
+    <t>OCHOA RUEDA, ASHLY SOFIA</t>
+  </si>
+  <si>
+    <t>PLANCHEZ URDANETA, GLEINNYS DE</t>
+  </si>
+  <si>
+    <t>ROLDAN GALLO, HALAN STIVEN</t>
+  </si>
+  <si>
+    <t>TABORDA GAVIRIA, JERONIMO</t>
+  </si>
+  <si>
+    <t>YU LUO, WENJIN</t>
+  </si>
+  <si>
+    <t>ZAPATA GONZALEZ, NYCHOLL</t>
+  </si>
+  <si>
+    <t>ALVAREZ QUINTERO, MARIA ISABEL</t>
+  </si>
+  <si>
+    <t>BEDOYA JARAMILLO, JUAN JOSE</t>
+  </si>
+  <si>
+    <t>BLANDON HENAO, ANDRES FELIPE</t>
+  </si>
+  <si>
+    <t>CANO VELASQUEZ, ANA SOFIA</t>
+  </si>
+  <si>
+    <t>CASTAÑEDA RESTREPO, MARIANA</t>
+  </si>
+  <si>
+    <t>CIRO RAMIREZ, MARIA ISABEL</t>
+  </si>
+  <si>
+    <t>COLORADO LOPEZ, EILEEN DAHIANA</t>
+  </si>
+  <si>
+    <t>CORREA AGUADO, DIEGO ALEJANDRO</t>
+  </si>
+  <si>
+    <t>GAÑAN LONDOÑO, JADED SOFIA</t>
+  </si>
+  <si>
+    <t>GUARINO COLMENARES, DAVID</t>
+  </si>
+  <si>
+    <t>HERRERA ESTRADA, MARIA ALEJANDRA</t>
+  </si>
+  <si>
+    <t>IDARRAGA SALAZAR, CRISTIAN DAVID</t>
+  </si>
+  <si>
+    <t>JARABA CAÑAS, SIMON</t>
+  </si>
+  <si>
+    <t>LOPEZ CARDONA, SULEIKA MICHEL</t>
+  </si>
+  <si>
+    <t>MARIN HERRERA, VALENTINA</t>
+  </si>
+  <si>
+    <t>MARTINEZ CANO, MATEO</t>
+  </si>
+  <si>
+    <t>NAVARRO FRANCO, LISMARY MILITZA</t>
+  </si>
+  <si>
+    <t>RAMIREZ ARTEAGA, JUAN MANUEL</t>
+  </si>
+  <si>
+    <t>RINCON FUENTES, MANUELA</t>
+  </si>
+  <si>
+    <t>RUIZ DOMINGUEZ, DAVID</t>
+  </si>
+  <si>
+    <t>SANCHEZ ARANGO, NICOL DAHIANA</t>
+  </si>
+  <si>
+    <t>SERNA GOEZ, MARLON</t>
+  </si>
+  <si>
+    <t>VELEZ VILLA, JUAN JOSE</t>
+  </si>
+  <si>
+    <t>PP2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1294,6 +1435,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1671,10 +1818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122C58AF-DAD1-4F23-B77B-FF91B1E85975}">
-  <dimension ref="A1:K581"/>
+  <dimension ref="A1:K627"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A572" workbookViewId="0">
-      <selection activeCell="C554" sqref="C554"/>
+    <sheetView tabSelected="1" topLeftCell="B507" workbookViewId="0">
+      <selection activeCell="I600" sqref="I600"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -22021,8 +22168,929 @@
         <v>409</v>
       </c>
     </row>
+    <row r="582" spans="1:11">
+      <c r="A582">
+        <v>1105</v>
+      </c>
+      <c r="B582" t="s">
+        <v>214</v>
+      </c>
+      <c r="C582" t="s">
+        <v>416</v>
+      </c>
+      <c r="E582">
+        <v>35.416666666666664</v>
+      </c>
+      <c r="J582">
+        <v>2024</v>
+      </c>
+      <c r="K582" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="583" spans="1:11">
+      <c r="A583">
+        <v>1105</v>
+      </c>
+      <c r="B583" t="s">
+        <v>215</v>
+      </c>
+      <c r="C583" t="s">
+        <v>417</v>
+      </c>
+      <c r="E583">
+        <v>56.25</v>
+      </c>
+      <c r="J583">
+        <v>2024</v>
+      </c>
+      <c r="K583" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="584" spans="1:11">
+      <c r="A584">
+        <v>1105</v>
+      </c>
+      <c r="B584" t="s">
+        <v>216</v>
+      </c>
+      <c r="C584" t="s">
+        <v>418</v>
+      </c>
+      <c r="E584">
+        <v>45.833333333333336</v>
+      </c>
+      <c r="J584">
+        <v>2024</v>
+      </c>
+      <c r="K584" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="585" spans="1:11">
+      <c r="A585">
+        <v>1105</v>
+      </c>
+      <c r="B585" t="s">
+        <v>217</v>
+      </c>
+      <c r="C585" t="s">
+        <v>419</v>
+      </c>
+      <c r="E585">
+        <v>56.25</v>
+      </c>
+      <c r="J585">
+        <v>2024</v>
+      </c>
+      <c r="K585" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="586" spans="1:11">
+      <c r="A586">
+        <v>1105</v>
+      </c>
+      <c r="B586" t="s">
+        <v>218</v>
+      </c>
+      <c r="C586" t="s">
+        <v>420</v>
+      </c>
+      <c r="E586">
+        <v>58.333333333333336</v>
+      </c>
+      <c r="J586">
+        <v>2024</v>
+      </c>
+      <c r="K586" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="587" spans="1:11">
+      <c r="A587">
+        <v>1105</v>
+      </c>
+      <c r="B587" t="s">
+        <v>219</v>
+      </c>
+      <c r="C587" t="s">
+        <v>421</v>
+      </c>
+      <c r="E587">
+        <v>35.416666666666664</v>
+      </c>
+      <c r="J587">
+        <v>2024</v>
+      </c>
+      <c r="K587" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="588" spans="1:11">
+      <c r="A588">
+        <v>1105</v>
+      </c>
+      <c r="B588" t="s">
+        <v>220</v>
+      </c>
+      <c r="C588" t="s">
+        <v>422</v>
+      </c>
+      <c r="E588">
+        <v>27.083333333333332</v>
+      </c>
+      <c r="J588">
+        <v>2024</v>
+      </c>
+      <c r="K588" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="589" spans="1:11">
+      <c r="A589">
+        <v>1105</v>
+      </c>
+      <c r="B589" t="s">
+        <v>221</v>
+      </c>
+      <c r="C589" t="s">
+        <v>423</v>
+      </c>
+      <c r="E589">
+        <v>29.166666666666668</v>
+      </c>
+      <c r="J589">
+        <v>2024</v>
+      </c>
+      <c r="K589" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="590" spans="1:11">
+      <c r="A590">
+        <v>1105</v>
+      </c>
+      <c r="B590" t="s">
+        <v>222</v>
+      </c>
+      <c r="C590" t="s">
+        <v>424</v>
+      </c>
+      <c r="E590">
+        <v>45.833333333333336</v>
+      </c>
+      <c r="J590">
+        <v>2024</v>
+      </c>
+      <c r="K590" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="591" spans="1:11">
+      <c r="A591">
+        <v>1105</v>
+      </c>
+      <c r="B591" t="s">
+        <v>223</v>
+      </c>
+      <c r="C591" t="s">
+        <v>425</v>
+      </c>
+      <c r="E591">
+        <v>43.75</v>
+      </c>
+      <c r="J591">
+        <v>2024</v>
+      </c>
+      <c r="K591" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="592" spans="1:11">
+      <c r="A592">
+        <v>1105</v>
+      </c>
+      <c r="B592" t="s">
+        <v>224</v>
+      </c>
+      <c r="C592" t="s">
+        <v>426</v>
+      </c>
+      <c r="E592">
+        <v>0</v>
+      </c>
+      <c r="J592">
+        <v>2024</v>
+      </c>
+      <c r="K592" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="593" spans="1:11">
+      <c r="A593">
+        <v>1105</v>
+      </c>
+      <c r="B593" t="s">
+        <v>225</v>
+      </c>
+      <c r="C593" t="s">
+        <v>427</v>
+      </c>
+      <c r="E593">
+        <v>35.416666666666664</v>
+      </c>
+      <c r="J593">
+        <v>2024</v>
+      </c>
+      <c r="K593" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="594" spans="1:11">
+      <c r="A594">
+        <v>1105</v>
+      </c>
+      <c r="B594" t="s">
+        <v>226</v>
+      </c>
+      <c r="C594" t="s">
+        <v>428</v>
+      </c>
+      <c r="E594">
+        <v>10.416666666666666</v>
+      </c>
+      <c r="J594">
+        <v>2024</v>
+      </c>
+      <c r="K594" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="595" spans="1:11">
+      <c r="A595">
+        <v>1105</v>
+      </c>
+      <c r="B595" t="s">
+        <v>227</v>
+      </c>
+      <c r="C595" t="s">
+        <v>429</v>
+      </c>
+      <c r="E595">
+        <v>50</v>
+      </c>
+      <c r="J595">
+        <v>2024</v>
+      </c>
+      <c r="K595" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="596" spans="1:11">
+      <c r="A596">
+        <v>1105</v>
+      </c>
+      <c r="B596" t="s">
+        <v>338</v>
+      </c>
+      <c r="C596" t="s">
+        <v>430</v>
+      </c>
+      <c r="E596">
+        <v>37.5</v>
+      </c>
+      <c r="J596">
+        <v>2024</v>
+      </c>
+      <c r="K596" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="597" spans="1:11">
+      <c r="A597">
+        <v>1105</v>
+      </c>
+      <c r="B597">
+        <v>4150805</v>
+      </c>
+      <c r="C597" t="s">
+        <v>431</v>
+      </c>
+      <c r="E597">
+        <v>47.916666666666664</v>
+      </c>
+      <c r="J597">
+        <v>2024</v>
+      </c>
+      <c r="K597" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="598" spans="1:11">
+      <c r="A598">
+        <v>1105</v>
+      </c>
+      <c r="B598" t="s">
+        <v>229</v>
+      </c>
+      <c r="C598" t="s">
+        <v>432</v>
+      </c>
+      <c r="E598">
+        <v>43.75</v>
+      </c>
+      <c r="J598">
+        <v>2024</v>
+      </c>
+      <c r="K598" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="599" spans="1:11">
+      <c r="A599">
+        <v>1105</v>
+      </c>
+      <c r="B599" t="s">
+        <v>230</v>
+      </c>
+      <c r="C599" t="s">
+        <v>433</v>
+      </c>
+      <c r="E599">
+        <v>35.416666666666664</v>
+      </c>
+      <c r="J599">
+        <v>2024</v>
+      </c>
+      <c r="K599" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="600" spans="1:11">
+      <c r="A600">
+        <v>1105</v>
+      </c>
+      <c r="B600" t="s">
+        <v>256</v>
+      </c>
+      <c r="C600" t="s">
+        <v>434</v>
+      </c>
+      <c r="E600">
+        <v>50</v>
+      </c>
+      <c r="J600">
+        <v>2024</v>
+      </c>
+      <c r="K600" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="601" spans="1:11">
+      <c r="A601">
+        <v>1105</v>
+      </c>
+      <c r="B601" t="s">
+        <v>231</v>
+      </c>
+      <c r="C601" t="s">
+        <v>435</v>
+      </c>
+      <c r="E601">
+        <v>47.916666666666664</v>
+      </c>
+      <c r="J601">
+        <v>2024</v>
+      </c>
+      <c r="K601" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="602" spans="1:11">
+      <c r="A602">
+        <v>1105</v>
+      </c>
+      <c r="B602" t="s">
+        <v>257</v>
+      </c>
+      <c r="C602" t="s">
+        <v>436</v>
+      </c>
+      <c r="E602">
+        <v>75</v>
+      </c>
+      <c r="J602">
+        <v>2024</v>
+      </c>
+      <c r="K602" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="603" spans="1:11">
+      <c r="A603">
+        <v>1105</v>
+      </c>
+      <c r="B603" t="s">
+        <v>232</v>
+      </c>
+      <c r="C603" t="s">
+        <v>437</v>
+      </c>
+      <c r="E603">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="J603">
+        <v>2024</v>
+      </c>
+      <c r="K603" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="604" spans="1:11">
+      <c r="A604">
+        <v>1105</v>
+      </c>
+      <c r="B604" t="s">
+        <v>405</v>
+      </c>
+      <c r="C604" t="s">
+        <v>438</v>
+      </c>
+      <c r="E604">
+        <v>22.916666666666668</v>
+      </c>
+      <c r="J604">
+        <v>2024</v>
+      </c>
+      <c r="K604" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="605" spans="1:11">
+      <c r="A605">
+        <v>1106</v>
+      </c>
+      <c r="B605" t="s">
+        <v>233</v>
+      </c>
+      <c r="C605" t="s">
+        <v>439</v>
+      </c>
+      <c r="E605">
+        <v>50</v>
+      </c>
+      <c r="J605">
+        <v>2024</v>
+      </c>
+      <c r="K605" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="606" spans="1:11">
+      <c r="A606">
+        <v>1106</v>
+      </c>
+      <c r="B606" t="s">
+        <v>234</v>
+      </c>
+      <c r="C606" t="s">
+        <v>440</v>
+      </c>
+      <c r="E606">
+        <v>45.833333333333336</v>
+      </c>
+      <c r="J606">
+        <v>2024</v>
+      </c>
+      <c r="K606" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="607" spans="1:11">
+      <c r="A607">
+        <v>1106</v>
+      </c>
+      <c r="B607" t="s">
+        <v>235</v>
+      </c>
+      <c r="C607" t="s">
+        <v>441</v>
+      </c>
+      <c r="E607">
+        <v>27.083333333333332</v>
+      </c>
+      <c r="J607">
+        <v>2024</v>
+      </c>
+      <c r="K607" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="608" spans="1:11">
+      <c r="A608">
+        <v>1106</v>
+      </c>
+      <c r="B608" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C608" t="s">
+        <v>442</v>
+      </c>
+      <c r="E608">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="J608">
+        <v>2024</v>
+      </c>
+      <c r="K608" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="609" spans="1:11">
+      <c r="A609">
+        <v>1106</v>
+      </c>
+      <c r="B609" t="s">
+        <v>237</v>
+      </c>
+      <c r="C609" t="s">
+        <v>443</v>
+      </c>
+      <c r="E609">
+        <v>39.583333333333336</v>
+      </c>
+      <c r="J609">
+        <v>2024</v>
+      </c>
+      <c r="K609" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="610" spans="1:11">
+      <c r="A610">
+        <v>1106</v>
+      </c>
+      <c r="B610" t="s">
+        <v>238</v>
+      </c>
+      <c r="C610" t="s">
+        <v>444</v>
+      </c>
+      <c r="E610">
+        <v>37.5</v>
+      </c>
+      <c r="J610">
+        <v>2024</v>
+      </c>
+      <c r="K610" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="611" spans="1:11">
+      <c r="A611">
+        <v>1106</v>
+      </c>
+      <c r="B611" t="s">
+        <v>239</v>
+      </c>
+      <c r="C611" t="s">
+        <v>445</v>
+      </c>
+      <c r="E611">
+        <v>25</v>
+      </c>
+      <c r="J611">
+        <v>2024</v>
+      </c>
+      <c r="K611" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="612" spans="1:11">
+      <c r="A612">
+        <v>1106</v>
+      </c>
+      <c r="B612" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C612" t="s">
+        <v>446</v>
+      </c>
+      <c r="E612">
+        <v>60.416666666666664</v>
+      </c>
+      <c r="J612">
+        <v>2024</v>
+      </c>
+      <c r="K612" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="613" spans="1:11">
+      <c r="A613">
+        <v>1106</v>
+      </c>
+      <c r="B613" t="s">
+        <v>241</v>
+      </c>
+      <c r="C613" t="s">
+        <v>447</v>
+      </c>
+      <c r="E613">
+        <v>0</v>
+      </c>
+      <c r="J613">
+        <v>2024</v>
+      </c>
+      <c r="K613" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="614" spans="1:11">
+      <c r="A614">
+        <v>1106</v>
+      </c>
+      <c r="B614" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C614" t="s">
+        <v>448</v>
+      </c>
+      <c r="E614">
+        <v>77.083333333333329</v>
+      </c>
+      <c r="J614">
+        <v>2024</v>
+      </c>
+      <c r="K614" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="615" spans="1:11">
+      <c r="A615">
+        <v>1106</v>
+      </c>
+      <c r="B615" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C615" t="s">
+        <v>449</v>
+      </c>
+      <c r="E615">
+        <v>56.25</v>
+      </c>
+      <c r="J615">
+        <v>2024</v>
+      </c>
+      <c r="K615" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="616" spans="1:11">
+      <c r="A616">
+        <v>1106</v>
+      </c>
+      <c r="B616" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C616" t="s">
+        <v>450</v>
+      </c>
+      <c r="E616">
+        <v>29.166666666666668</v>
+      </c>
+      <c r="J616">
+        <v>2024</v>
+      </c>
+      <c r="K616" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="617" spans="1:11">
+      <c r="A617">
+        <v>1106</v>
+      </c>
+      <c r="B617" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C617" t="s">
+        <v>451</v>
+      </c>
+      <c r="E617">
+        <v>47.916666666666664</v>
+      </c>
+      <c r="J617">
+        <v>2024</v>
+      </c>
+      <c r="K617" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="618" spans="1:11">
+      <c r="A618">
+        <v>1106</v>
+      </c>
+      <c r="B618" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C618" t="s">
+        <v>452</v>
+      </c>
+      <c r="E618">
+        <v>50</v>
+      </c>
+      <c r="J618">
+        <v>2024</v>
+      </c>
+      <c r="K618" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="619" spans="1:11">
+      <c r="A619">
+        <v>1106</v>
+      </c>
+      <c r="B619" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C619" t="s">
+        <v>453</v>
+      </c>
+      <c r="E619">
+        <v>31.25</v>
+      </c>
+      <c r="J619">
+        <v>2024</v>
+      </c>
+      <c r="K619" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="620" spans="1:11">
+      <c r="A620">
+        <v>1106</v>
+      </c>
+      <c r="B620" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C620" t="s">
+        <v>454</v>
+      </c>
+      <c r="E620">
+        <v>39.583333333333336</v>
+      </c>
+      <c r="J620">
+        <v>2024</v>
+      </c>
+      <c r="K620" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="621" spans="1:11">
+      <c r="A621">
+        <v>1106</v>
+      </c>
+      <c r="B621" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C621" t="s">
+        <v>455</v>
+      </c>
+      <c r="E621">
+        <v>37.5</v>
+      </c>
+      <c r="J621">
+        <v>2024</v>
+      </c>
+      <c r="K621" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="622" spans="1:11">
+      <c r="A622">
+        <v>1106</v>
+      </c>
+      <c r="B622" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C622" t="s">
+        <v>456</v>
+      </c>
+      <c r="E622">
+        <v>29.166666666666668</v>
+      </c>
+      <c r="J622">
+        <v>2024</v>
+      </c>
+      <c r="K622" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="623" spans="1:11">
+      <c r="A623">
+        <v>1106</v>
+      </c>
+      <c r="B623" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C623" t="s">
+        <v>457</v>
+      </c>
+      <c r="E623">
+        <v>29.166666666666668</v>
+      </c>
+      <c r="J623">
+        <v>2024</v>
+      </c>
+      <c r="K623" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="624" spans="1:11">
+      <c r="A624">
+        <v>1106</v>
+      </c>
+      <c r="B624" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C624" t="s">
+        <v>458</v>
+      </c>
+      <c r="E624">
+        <v>72.916666666666671</v>
+      </c>
+      <c r="J624">
+        <v>2024</v>
+      </c>
+      <c r="K624" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="625" spans="1:11">
+      <c r="A625">
+        <v>1106</v>
+      </c>
+      <c r="B625" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C625" t="s">
+        <v>459</v>
+      </c>
+      <c r="E625">
+        <v>33.333333333333336</v>
+      </c>
+      <c r="J625">
+        <v>2024</v>
+      </c>
+      <c r="K625" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="626" spans="1:11">
+      <c r="A626">
+        <v>1106</v>
+      </c>
+      <c r="B626" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C626" t="s">
+        <v>460</v>
+      </c>
+      <c r="E626">
+        <v>31.25</v>
+      </c>
+      <c r="J626">
+        <v>2024</v>
+      </c>
+      <c r="K626" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="627" spans="1:11">
+      <c r="A627">
+        <v>1106</v>
+      </c>
+      <c r="B627" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C627" t="s">
+        <v>461</v>
+      </c>
+      <c r="E627">
+        <v>31.25</v>
+      </c>
+      <c r="J627">
+        <v>2024</v>
+      </c>
+      <c r="K627" t="s">
+        <v>462</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K581" xr:uid="{F320DEFD-E675-4434-9FAA-F3C254001E23}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" copies="2" r:id="rId1"/>
 </worksheet>

</xml_diff>